<commit_message>
Added and amended some dose-response curve functions, amended plot.IL and plotmodelIL. No E, W, or N
</commit_message>
<xml_diff>
--- a/data-raw/alternatives.xlsx
+++ b/data-raw/alternatives.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\rcode2\biology\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBD2BF4-05E1-4362-8D6C-0A2DC604622B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F292D008-B968-4542-84AC-1DA797F339DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{65B50F89-D289-4F14-A1B5-F527CF9F2E44}"/>
+    <workbookView xWindow="-29952" yWindow="144" windowWidth="13728" windowHeight="16632" xr2:uid="{65B50F89-D289-4F14-A1B5-F527CF9F2E44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>steep</t>
   </si>
   <si>
-    <t>delta</t>
-  </si>
-  <si>
     <t>invlog</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>doseresponse</t>
+  </si>
+  <si>
+    <t>L95</t>
   </si>
 </sst>
 </file>
@@ -3346,16 +3346,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>521970</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>118110</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3683,7 +3683,7 @@
   <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C8" sqref="C8:C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3740,10 +3740,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -3763,13 +3763,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3781,7 +3781,7 @@
         <v>4.9999996141975611</v>
       </c>
       <c r="C8">
-        <f>$E$1/(1+EXP(LN(19)*(A8-$E$2)/$E$3))</f>
+        <f>$E$1/(1+EXP(LN(19)*(A8-$E$2)/($E$3-$E$2)))</f>
         <v>4.9358494559677295</v>
       </c>
       <c r="D8">
@@ -3802,7 +3802,7 @@
         <v>4.9999938271681144</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C72" si="1">$E$1/(1+EXP(LN(19)*(A9-$E$2)/$E$3))</f>
+        <f t="shared" ref="C9:C72" si="1">$E$1/(1+EXP(LN(19)*(A9-$E$2)/($E$3-$E$2)))</f>
         <v>4.9310167335500275</v>
       </c>
       <c r="D9">
@@ -5146,7 +5146,7 @@
         <v>2.029138427823546</v>
       </c>
       <c r="C73">
-        <f t="shared" ref="C73:C136" si="6">$E$1/(1+EXP(LN(19)*(A73-$E$2)/$E$3))</f>
+        <f t="shared" ref="C73:C136" si="6">$E$1/(1+EXP(LN(19)*(A73-$E$2)/($E$3-$E$2)))</f>
         <v>1.9567205147674553</v>
       </c>
       <c r="D73">
@@ -6490,7 +6490,7 @@
         <v>0.21703453126569988</v>
       </c>
       <c r="C137">
-        <f t="shared" ref="C137" si="11">$E$1/(1+EXP(LN(19)*(A137-$E$2)/$E$3))</f>
+        <f t="shared" ref="C137" si="11">$E$1/(1+EXP(LN(19)*(A137-$E$2)/($E$3-$E$2)))</f>
         <v>2.8750589300412025E-2</v>
       </c>
       <c r="D137">

</xml_diff>